<commit_message>
Realização de teste,Definições armazenadas no gitignore para futuras alterações, organização estrutura do programa
</commit_message>
<xml_diff>
--- a/dist/Comprovantes/comprovantes_funcionario.xlsx
+++ b/dist/Comprovantes/comprovantes_funcionario.xlsx
@@ -424,7 +424,7 @@
     <col width="17" customWidth="1" min="1" max="1"/>
     <col width="19" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="39" customWidth="1" min="4" max="4"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -458,22 +458,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mateus Esteves:</t>
+          <t>Você</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>13:05, 25/03/2025</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 292,00</t>
+          <t>R$ 200,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RAFAEL TRUYTS</t>
+          <t>COMERCIO DE POLPAS SOUZA E DIAS LTD...</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>13:32, 25/03/2025</t>
+          <t>20:28, 25/03/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">

</xml_diff>